<commit_message>
pase datos de excel
</commit_message>
<xml_diff>
--- a/TP3/datos.xlsx
+++ b/TP3/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa-m\InformesElectro\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAF468B2-70FD-47CC-A871-C3DCEEE4C241}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF71D981-4CD3-4D4D-8F14-53837D600B11}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" xr2:uid="{A3A859C2-6CC3-49AB-87AC-DEFDF2AC605D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>U</t>
   </si>
@@ -90,17 +90,37 @@
     <t>B</t>
   </si>
   <si>
-    <t>0*</t>
+    <t>Xl</t>
+  </si>
+  <si>
+    <t>Xc con 10uF</t>
+  </si>
+  <si>
+    <t>Xc con 20uF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,9 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,15 +465,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A65BBA-3DAF-4E23-8D70-559EA97E0D9E}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -499,96 +523,154 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>101</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>101</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.34</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0.3</v>
       </c>
-      <c r="I2">
-        <v>0.44</v>
-      </c>
-      <c r="J2">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J2" s="1">
         <f>D2-I2</f>
         <v>31.56</v>
       </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2">
+      <c r="K2" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <f>C2*B2</f>
         <v>34.340000000000003</v>
       </c>
+      <c r="N2">
+        <f>COS(ASIN(K2/L2))</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <f>(C2/B2)*(D2/L2)</f>
+        <v>3.1369473581021471E-3</v>
+      </c>
+      <c r="P2">
+        <f>(C2/B2)*(-K2/L2)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>101</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>101</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.74</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>12</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.72499999999999998</v>
       </c>
-      <c r="I3">
-        <v>0.44</v>
-      </c>
-      <c r="J3">
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J3" s="1">
         <f t="shared" ref="J3:J8" si="0">D3-I3</f>
         <v>11.56</v>
       </c>
-      <c r="K3">
-        <v>73.376999999999995</v>
-      </c>
-      <c r="L3">
+      <c r="K3" s="1">
+        <v>73.739999999999995</v>
+      </c>
+      <c r="L3" s="1">
         <f t="shared" ref="L3:L8" si="1">C3*B3</f>
         <v>74.739999999999995</v>
       </c>
+      <c r="N3">
+        <f>COS(ASIN(K3/L3))</f>
+        <v>0.16303501430803102</v>
+      </c>
+      <c r="O3">
+        <f>(C3/B3)*(D3/L3)</f>
+        <v>1.1763552592883053E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P8" si="2">(C3/B3)*(-K3/L3)</f>
+        <v>-7.2287030683266347E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>101</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2">
         <v>0.38</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
         <v>0.32500000000000001</v>
       </c>
-      <c r="I4">
-        <v>0.44</v>
-      </c>
-      <c r="J4">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J4" s="1">
         <f t="shared" si="0"/>
         <v>1.56</v>
       </c>
-      <c r="K4" s="1">
-        <v>105.625</v>
-      </c>
-      <c r="L4">
+      <c r="K4" s="3">
+        <v>-33.619999999999997</v>
+      </c>
+      <c r="L4" s="1">
         <f t="shared" si="1"/>
         <v>38.380000000000003</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N8" si="3">COS(ASIN(K4/L4))</f>
+        <v>0.4823527447798287</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O8" si="4">(C4/B4)*(D4/L4)</f>
+        <v>1.9605920988138414E-4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>3.2957553181060671E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -598,8 +680,8 @@
       <c r="B5">
         <v>101</v>
       </c>
-      <c r="C5">
-        <v>1.06</v>
+      <c r="C5" s="2">
+        <v>0.82599999999999996</v>
       </c>
       <c r="D5">
         <v>42</v>
@@ -609,6 +691,9 @@
       </c>
       <c r="F5">
         <v>0.72499999999999998</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0.44</v>
@@ -617,9 +702,24 @@
         <f t="shared" si="0"/>
         <v>41.56</v>
       </c>
+      <c r="K5">
+        <v>73.739999999999995</v>
+      </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>107.06</v>
+        <v>83.426000000000002</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>0.4676814142837854</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>4.1172434075090678E-3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>-7.2287030683266347E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -629,14 +729,17 @@
       <c r="B6">
         <v>101</v>
       </c>
-      <c r="C6">
-        <v>0.66</v>
+      <c r="C6" s="2">
+        <v>0.45629999999999998</v>
       </c>
       <c r="D6">
         <v>31.5</v>
       </c>
       <c r="E6">
         <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0.32500000000000001</v>
@@ -648,9 +751,24 @@
         <f t="shared" si="0"/>
         <v>31.06</v>
       </c>
+      <c r="K6" s="3">
+        <v>-33.619999999999997</v>
+      </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>66.66</v>
+        <v>46.086300000000001</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>0.68397978939327164</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>3.0879325556318012E-3</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>3.2957553181060676E-3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -660,11 +778,14 @@
       <c r="B7">
         <v>101</v>
       </c>
-      <c r="C7">
-        <v>1.1000000000000001</v>
+      <c r="C7" s="2">
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>12</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0.72499999999999998</v>
@@ -679,9 +800,24 @@
         <f t="shared" si="0"/>
         <v>11.56</v>
       </c>
+      <c r="K7">
+        <v>40.119999999999997</v>
+      </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>111.10000000000001</v>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>0.11753021582637106</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>1.1763552592883048E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>-3.9329477502205654E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -691,8 +827,8 @@
       <c r="B8">
         <v>101</v>
       </c>
-      <c r="C8">
-        <v>1.55</v>
+      <c r="C8" s="2">
+        <v>0.57999999999999996</v>
       </c>
       <c r="D8">
         <v>42</v>
@@ -713,9 +849,435 @@
         <f t="shared" si="0"/>
         <v>41.56</v>
       </c>
+      <c r="K8">
+        <v>40.119999999999997</v>
+      </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>156.55000000000001</v>
+        <v>58.58</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>0.72866021454954755</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>4.1172434075090678E-3</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>-3.9329477502205662E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>318.31</v>
+      </c>
+      <c r="B13">
+        <v>140.30000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="D18" s="1">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" ref="J18:J24" si="5">D18-I18</f>
+        <v>31.56</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" ref="L18:L24" si="6">C18*B18</f>
+        <v>34.340000000000003</v>
+      </c>
+      <c r="N18">
+        <f>COS(ASIN(K18/L18))</f>
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18:O24" si="7">(C18/B18)*(D18/L18)</f>
+        <v>3.1369473581021471E-3</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P24" si="8">(C18/B18)*(-K18/L18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>101</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D19" s="1">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="5"/>
+        <v>11.56</v>
+      </c>
+      <c r="K19" s="1">
+        <v>73.739999999999995</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="6"/>
+        <v>74.739999999999995</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:N24" si="9">COS(ASIN(K19/L19))</f>
+        <v>0.16303501430803102</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>1.1763552592883053E-3</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="8"/>
+        <v>-7.2287030683266347E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <v>101</v>
+      </c>
+      <c r="C20" s="2">
+        <f>0.35*2</f>
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="5"/>
+        <v>1.56</v>
+      </c>
+      <c r="K20" s="3">
+        <v>-67.239999999999995</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="6"/>
+        <v>70.699999999999989</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="9"/>
+        <v>0.30900374748766457</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="7"/>
+        <v>1.9605920988138419E-4</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="8"/>
+        <v>6.591510636212136E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>101</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="D21">
+        <v>42</v>
+      </c>
+      <c r="E21">
+        <v>0.3</v>
+      </c>
+      <c r="F21">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0.44</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>41.56</v>
+      </c>
+      <c r="K21">
+        <v>73.739999999999995</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="6"/>
+        <v>83.426000000000002</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="9"/>
+        <v>0.4676814142837854</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="7"/>
+        <v>4.1172434075090678E-3</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="8"/>
+        <v>-7.2287030683266347E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="D22">
+        <v>31.5</v>
+      </c>
+      <c r="E22">
+        <v>0.3</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="I22">
+        <v>0.44</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>31.06</v>
+      </c>
+      <c r="K22">
+        <v>-67.239999999999995</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="6"/>
+        <v>71.709999999999994</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="9"/>
+        <v>0.34753881391769981</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="7"/>
+        <v>3.0879325556318008E-3</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="8"/>
+        <v>6.5915106362121351E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>101</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="I23">
+        <v>0.44</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>11.56</v>
+      </c>
+      <c r="K23" s="3">
+        <v>6.4969999999999999</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="6"/>
+        <v>12.12</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="9"/>
+        <v>0.84418235686233045</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="7"/>
+        <v>1.1763552592883053E-3</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="8"/>
+        <v>-6.3689834329967645E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>101</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="D24">
+        <v>42</v>
+      </c>
+      <c r="E24">
+        <v>0.3</v>
+      </c>
+      <c r="F24">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="I24">
+        <v>0.44</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="5"/>
+        <v>41.56</v>
+      </c>
+      <c r="K24" s="3">
+        <v>6.4969999999999999</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>44.44</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="9"/>
+        <v>0.98925547872524999</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="7"/>
+        <v>4.1172434075090686E-3</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="8"/>
+        <v>-6.3689834329967655E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>159.155</v>
+      </c>
+      <c r="B27">
+        <v>140.30000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>